<commit_message>
update testsuite.py update run.py update module.py add requirements.txt
</commit_message>
<xml_diff>
--- a/data/testsuite.xlsx
+++ b/data/testsuite.xlsx
@@ -4,22 +4,48 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="11620"/>
+    <workbookView windowWidth="28000" windowHeight="11580"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestSuite" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
+  <si>
+    <t>序号</t>
+  </si>
+  <si>
+    <t>执行</t>
+  </si>
+  <si>
+    <t>测试场景</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>userregister</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -32,6 +58,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -60,9 +101,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -78,15 +150,43 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -95,80 +195,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,91 +209,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,91 +389,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -382,30 +408,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -444,7 +446,33 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -466,11 +494,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -479,145 +505,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -947,14 +973,48 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>

</xml_diff>